<commit_message>
Updates after first build, intermediate check in
</commit_message>
<xml_diff>
--- a/Li-ion 5A Boost 1A Charge Protect/Gerbers/Bill of Materials.xlsx
+++ b/Li-ion 5A Boost 1A Charge Protect/Gerbers/Bill of Materials.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Li-ion 5A Boost 1A Charge Prote" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Li-ion 5A Boost 1A Charge Prote'!$A$10:$L$37</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -51,9 +54,6 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Reference(s)</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -640,6 +640,9 @@
   </si>
   <si>
     <t>W1, W2, W3, W4, W5, W6, W7, W8</t>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1126,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1131,6 +1134,22 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1456,22 +1475,23 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="30" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1516,7 +1536,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1526,35 +1546,35 @@
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1564,35 +1584,35 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" t="s">
-        <v>27</v>
-      </c>
       <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
         <v>28</v>
-      </c>
-      <c r="L11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1602,35 +1622,35 @@
       <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>200</v>
+      <c r="C12" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
         <v>31</v>
       </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
         <v>32</v>
-      </c>
-      <c r="K12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1640,35 +1660,35 @@
       <c r="B13" s="2">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
-        <v>201</v>
+      <c r="C13" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>36</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>38</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>39</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
         <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1678,35 +1698,35 @@
       <c r="B14" s="2">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
-        <v>202</v>
+      <c r="C14" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
         <v>43</v>
       </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
         <v>44</v>
-      </c>
-      <c r="K14" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1716,35 +1736,35 @@
       <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
         <v>48</v>
       </c>
-      <c r="I15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
         <v>49</v>
-      </c>
-      <c r="K15" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1754,35 +1774,35 @@
       <c r="B16" s="2">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
         <v>53</v>
       </c>
-      <c r="I16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
         <v>54</v>
-      </c>
-      <c r="K16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1792,35 +1812,35 @@
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
         <v>57</v>
       </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
         <v>58</v>
       </c>
-      <c r="I17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
         <v>59</v>
-      </c>
-      <c r="K17" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1830,35 +1850,35 @@
       <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
         <v>62</v>
       </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" t="s">
         <v>63</v>
       </c>
-      <c r="I18" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s">
         <v>64</v>
-      </c>
-      <c r="K18" t="s">
-        <v>28</v>
-      </c>
-      <c r="L18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1868,35 +1888,35 @@
       <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>67</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>68</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>69</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>71</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" t="s">
         <v>72</v>
-      </c>
-      <c r="J19" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" t="s">
-        <v>28</v>
-      </c>
-      <c r="L19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1906,35 +1926,35 @@
       <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
         <v>74</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>75</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>76</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>77</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>78</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" t="s">
         <v>79</v>
-      </c>
-      <c r="I20" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" t="s">
-        <v>82</v>
-      </c>
-      <c r="K20" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1944,35 +1964,35 @@
       <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>84</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>85</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>86</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>87</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>88</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>89</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
         <v>90</v>
-      </c>
-      <c r="K21" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1982,35 +2002,35 @@
       <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
-        <v>203</v>
+      <c r="C22" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="D22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" t="s">
         <v>92</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>93</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>94</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>95</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>96</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>97</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" t="s">
         <v>98</v>
-      </c>
-      <c r="K22" t="s">
-        <v>28</v>
-      </c>
-      <c r="L22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2020,35 +2040,35 @@
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
-        <v>204</v>
+      <c r="C23" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>101</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" t="s">
         <v>102</v>
       </c>
-      <c r="I23" t="s">
-        <v>97</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" t="s">
         <v>103</v>
-      </c>
-      <c r="K23" t="s">
-        <v>28</v>
-      </c>
-      <c r="L23" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2058,35 +2078,35 @@
       <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="6">
+        <v>330</v>
+      </c>
+      <c r="E24" t="s">
         <v>105</v>
       </c>
-      <c r="D24">
-        <v>330</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
         <v>106</v>
       </c>
-      <c r="F24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>107</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>108</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>109</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" t="s">
         <v>110</v>
-      </c>
-      <c r="K24" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2096,73 +2116,73 @@
       <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" t="s">
         <v>113</v>
       </c>
-      <c r="E25" t="s">
+      <c r="I25" t="s">
+        <v>108</v>
+      </c>
+      <c r="J25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>16</v>
+      </c>
+      <c r="B26" s="7">
+        <v>5</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" t="s">
-        <v>107</v>
-      </c>
-      <c r="H25" t="s">
-        <v>114</v>
-      </c>
-      <c r="I25" t="s">
-        <v>109</v>
-      </c>
-      <c r="J25" t="s">
-        <v>115</v>
-      </c>
-      <c r="K25" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>205</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="H26" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E26" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="I26" t="s">
-        <v>109</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="K26" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2172,35 +2192,35 @@
       <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
         <v>121</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" t="s">
         <v>122</v>
       </c>
-      <c r="E27" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" t="s">
-        <v>107</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
+        <v>108</v>
+      </c>
+      <c r="J27" t="s">
         <v>123</v>
       </c>
-      <c r="I27" t="s">
-        <v>109</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" t="s">
         <v>124</v>
-      </c>
-      <c r="K27" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2210,35 +2230,35 @@
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
         <v>126</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" t="s">
         <v>127</v>
       </c>
-      <c r="E28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" t="s">
-        <v>107</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
+        <v>108</v>
+      </c>
+      <c r="J28" t="s">
         <v>128</v>
       </c>
-      <c r="I28" t="s">
-        <v>109</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" t="s">
         <v>129</v>
-      </c>
-      <c r="K28" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2248,35 +2268,35 @@
       <c r="B29" s="2">
         <v>1</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="s">
         <v>131</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" t="s">
         <v>132</v>
       </c>
-      <c r="E29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
+        <v>108</v>
+      </c>
+      <c r="J29" t="s">
         <v>133</v>
       </c>
-      <c r="I29" t="s">
-        <v>109</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" t="s">
         <v>134</v>
-      </c>
-      <c r="K29" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2286,35 +2306,35 @@
       <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" t="s">
         <v>136</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" t="s">
         <v>137</v>
       </c>
-      <c r="E30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" t="s">
-        <v>107</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
+        <v>108</v>
+      </c>
+      <c r="J30" t="s">
         <v>138</v>
       </c>
-      <c r="I30" t="s">
-        <v>109</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" t="s">
         <v>139</v>
-      </c>
-      <c r="K30" t="s">
-        <v>28</v>
-      </c>
-      <c r="L30" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2324,35 +2344,35 @@
       <c r="B31" s="2">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" t="s">
         <v>141</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" t="s">
         <v>142</v>
       </c>
-      <c r="E31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" t="s">
-        <v>107</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
+        <v>108</v>
+      </c>
+      <c r="J31" t="s">
         <v>143</v>
       </c>
-      <c r="I31" t="s">
-        <v>109</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" t="s">
         <v>144</v>
-      </c>
-      <c r="K31" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2362,35 +2382,35 @@
       <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
         <v>146</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>147</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>148</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>149</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>150</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>151</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>152</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" t="s">
         <v>153</v>
-      </c>
-      <c r="K32" t="s">
-        <v>28</v>
-      </c>
-      <c r="L32" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2400,35 +2420,35 @@
       <c r="B33" s="2">
         <v>1</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33" t="s">
         <v>155</v>
       </c>
-      <c r="D33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
         <v>156</v>
       </c>
-      <c r="F33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>157</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>158</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>159</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" t="s">
         <v>160</v>
-      </c>
-      <c r="K33" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2438,35 +2458,35 @@
       <c r="B34" s="2">
         <v>1</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
         <v>162</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>163</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>164</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>165</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>166</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>167</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>168</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" t="s">
         <v>169</v>
-      </c>
-      <c r="K34" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2476,35 +2496,35 @@
       <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" t="s">
         <v>171</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>172</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>173</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>174</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>175</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" t="s">
         <v>176</v>
-      </c>
-      <c r="I35" t="s">
-        <v>72</v>
-      </c>
-      <c r="J35" t="s">
-        <v>172</v>
-      </c>
-      <c r="K35" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2514,35 +2534,35 @@
       <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" t="s">
         <v>178</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>179</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>180</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>181</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>182</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>183</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>184</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" t="s">
         <v>185</v>
-      </c>
-      <c r="K36" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2552,77 +2572,77 @@
       <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
         <v>187</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>188</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>189</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>190</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>191</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
+        <v>167</v>
+      </c>
+      <c r="J37" t="s">
+        <v>187</v>
+      </c>
+      <c r="K37" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" t="s">
         <v>192</v>
       </c>
-      <c r="I37" t="s">
-        <v>168</v>
-      </c>
-      <c r="J37" t="s">
-        <v>188</v>
-      </c>
-      <c r="K37" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>28</v>
       </c>
       <c r="B38" s="2">
         <v>8</v>
       </c>
-      <c r="C38" t="s">
-        <v>206</v>
+      <c r="C38" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="D38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" t="s">
         <v>194</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>195</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>196</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>197</v>
       </c>
-      <c r="H38" t="s">
-        <v>198</v>
-      </c>
       <c r="I38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>